<commit_message>
Actualización de manual de usuario
</commit_message>
<xml_diff>
--- a/data/info.xlsx
+++ b/data/info.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
@@ -473,31 +473,54 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>LUCAS CORTES</t>
+          <t>LUCAS</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>221</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>100000</v>
+        <v>50000</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2020/12/09, 18:55:05</t>
+          <t>2021/01/07, 12:31:19</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n"/>
-      <c r="B3" s="1" t="n"/>
-      <c r="C3" s="1" t="n"/>
-      <c r="D3" s="1" t="n"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>LUCAS CORTES</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>221</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="n">
+        <v>100000</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2020/12/09, 18:55:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n"/>
+      <c r="B4" s="1" t="n"/>
+      <c r="C4" s="1" t="n"/>
+      <c r="D4" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>